<commit_message>
update index data/returns to include HFRX AR Index
</commit_message>
<xml_diff>
--- a/data/time_series/index_returns.xlsx
+++ b/data/time_series/index_returns.xlsx
@@ -49,10 +49,10 @@
     <t>HFRX MACRO/CTA</t>
   </si>
   <si>
-    <t>HFRI MACRO</t>
+    <t>HF MACRO</t>
   </si>
   <si>
-    <t>SG TREND</t>
+    <t>TREND</t>
   </si>
   <si>
     <t>ALT RISK</t>
@@ -473,7 +473,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ALM180"/>
+  <dimension ref="A1:ALM181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -13553,7 +13553,7 @@
         <v>0.0277348443081904</v>
       </c>
       <c r="N174" s="1">
-        <v>0.0705852750942515</v>
+        <v>0.07058499551981989</v>
       </c>
       <c r="O174" s="1">
         <v>0.005875983963948173</v>
@@ -13630,7 +13630,7 @@
         <v>-0.001894176692981087</v>
       </c>
       <c r="N175" s="1">
-        <v>-0.002012357746336901</v>
+        <v>-0.002012097130104529</v>
       </c>
       <c r="O175" s="1">
         <v>0</v>
@@ -13704,10 +13704,10 @@
         <v>0.01373001390686412</v>
       </c>
       <c r="M176" s="1">
-        <v>-0.008443637358162892</v>
+        <v>-0.004234113832479403</v>
       </c>
       <c r="N176" s="1">
-        <v>0.02568221490655964</v>
+        <v>0.02568247657480471</v>
       </c>
       <c r="O176" s="1">
         <v>0</v>
@@ -13725,7 +13725,7 @@
         <v>0.5649993364820423</v>
       </c>
       <c r="T176" s="1">
-        <v>0.00529394343254852</v>
+        <v>0</v>
       </c>
       <c r="U176" s="1">
         <v>-0.08784248849818266</v>
@@ -13781,10 +13781,10 @@
         <v>-0.01484453678225639</v>
       </c>
       <c r="M177" s="1">
-        <v>-0.008030591048697189</v>
+        <v>-0.004227422915525914</v>
       </c>
       <c r="N177" s="1">
-        <v>-0.04407516644424769</v>
+        <v>-0.0440746449675008</v>
       </c>
       <c r="O177" s="1">
         <v>0</v>
@@ -13858,10 +13858,10 @@
         <v>0.0124522075099609</v>
       </c>
       <c r="M178" s="1">
-        <v>0.0130032985102233</v>
+        <v>-0.008030591048697189</v>
       </c>
       <c r="N178" s="1">
-        <v>0.03988693936721921</v>
+        <v>0.03991546346575769</v>
       </c>
       <c r="O178" s="1">
         <v>0</v>
@@ -13879,7 +13879,7 @@
         <v>0.1439047713525086</v>
       </c>
       <c r="T178" s="1">
-        <v>0</v>
+        <v>0.00529394343254852</v>
       </c>
       <c r="U178" s="1">
         <v>-0.03723930630118</v>
@@ -13935,10 +13935,10 @@
         <v>0.02985323814218255</v>
       </c>
       <c r="M179" s="1">
-        <v>0.01291285282918109</v>
+        <v>0.03031856333458149</v>
       </c>
       <c r="N179" s="1">
-        <v>0.057616721583853</v>
+        <v>0.0575868652098519</v>
       </c>
       <c r="O179" s="1">
         <v>0</v>
@@ -14012,7 +14012,7 @@
         <v>0.00146676239221244</v>
       </c>
       <c r="M180" s="1">
-        <v>0.008188497599453504</v>
+        <v>0.005376809760581303</v>
       </c>
       <c r="N180" s="1">
         <v>0.001892027978815491</v>
@@ -14051,13 +14051,90 @@
         <v>0.0005633562374631751</v>
       </c>
     </row>
+    <row r="181" spans="1:25">
+      <c r="A181" s="3">
+        <v>44895</v>
+      </c>
+      <c r="B181" s="1">
+        <v>0.0971428571428572</v>
+      </c>
+      <c r="C181" s="1">
+        <v>0.09077890818239998</v>
+      </c>
+      <c r="D181" s="1">
+        <v>0.06320955119635219</v>
+      </c>
+      <c r="E181" s="1">
+        <v>0.05375286029369986</v>
+      </c>
+      <c r="F181" s="1">
+        <v>0.07597591964118222</v>
+      </c>
+      <c r="G181" s="1">
+        <v>0.02150348997191442</v>
+      </c>
+      <c r="H181" s="1">
+        <v>0.1108742857142857</v>
+      </c>
+      <c r="I181" s="1">
+        <v>0.1463521033767214</v>
+      </c>
+      <c r="J181" s="1">
+        <v>0.01109882463139722</v>
+      </c>
+      <c r="K181" s="1">
+        <v>0.01871794686844064</v>
+      </c>
+      <c r="L181" s="1">
+        <v>-0.02390404464760609</v>
+      </c>
+      <c r="M181" s="1">
+        <v>-0.0201499607198482</v>
+      </c>
+      <c r="N181" s="1">
+        <v>-0.06032641182414533</v>
+      </c>
+      <c r="O181" s="1">
+        <v>0</v>
+      </c>
+      <c r="P181" s="1">
+        <v>0.0582618546690401</v>
+      </c>
+      <c r="Q181" s="1">
+        <v>0</v>
+      </c>
+      <c r="R181" s="1">
+        <v>0.04375997841006241</v>
+      </c>
+      <c r="S181" s="1">
+        <v>0.05340392030250962</v>
+      </c>
+      <c r="T181" s="1">
+        <v>0.01820209087747293</v>
+      </c>
+      <c r="U181" s="1">
+        <v>0.07455088815016286</v>
+      </c>
+      <c r="V181" s="1">
+        <v>0.05015475492350419</v>
+      </c>
+      <c r="W181" s="1">
+        <v>0.06438188494492048</v>
+      </c>
+      <c r="X181" s="1">
+        <v>0.05862550994208782</v>
+      </c>
+      <c r="Y181" s="1">
+        <v>-0.00846264747784109</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A180">
+  <conditionalFormatting sqref="A1:A181">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:Y180">
+  <conditionalFormatting sqref="B2:Y181">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>

</xml_diff>